<commit_message>
Modularized Jupyter notebook and added documentation 04222021
</commit_message>
<xml_diff>
--- a/Documentation/Recursive Approach diagram.xlsx
+++ b/Documentation/Recursive Approach diagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vdeshpande\Desktop\Del_Project-Takeda\Site_Master_Repo\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B8A89F-A60D-467C-BAA2-78186E03822A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A15220-C8B2-48E8-93CC-3B2FBB25EBEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{4E33DFAF-8DE4-4DA1-9A7B-6EFC66B427C2}"/>
   </bookViews>
@@ -35,48 +35,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
-    <t>Mini-Batch
-1</t>
-  </si>
-  <si>
-    <t>Mini-Batch
-2</t>
-  </si>
-  <si>
-    <t>Mini-Batch
-3</t>
-  </si>
-  <si>
-    <t>Mini-Batch
-4</t>
-  </si>
-  <si>
-    <t>Mini-Batch
-5</t>
-  </si>
-  <si>
     <t>Depth=0</t>
   </si>
   <si>
     <t>Depth=1</t>
   </si>
   <si>
-    <t>Cross Ref [1][2][3][4]</t>
-  </si>
-  <si>
     <t>Depth=2</t>
   </si>
   <si>
-    <t>Cross Ref [1][2][3][4][5]</t>
-  </si>
-  <si>
     <t>Depth=3</t>
-  </si>
-  <si>
-    <t>Cross Ref [1][2]</t>
-  </si>
-  <si>
-    <t>Cross Ref [3][4]</t>
   </si>
   <si>
     <t>Cross Ref [5]</t>
@@ -100,10 +68,6 @@
     <t>Master 2</t>
   </si>
   <si>
-    <t xml:space="preserve">Master
-[1][2][3][4] </t>
-  </si>
-  <si>
     <t>Master 3</t>
   </si>
   <si>
@@ -117,19 +81,55 @@
 [5]</t>
   </si>
   <si>
-    <t>Master
-[3][4]</t>
+    <t>Mini Batch
+1</t>
+  </si>
+  <si>
+    <t>Mini Batch
+2</t>
+  </si>
+  <si>
+    <t>Mini Batch
+3</t>
+  </si>
+  <si>
+    <t>Mini Batch
+4</t>
+  </si>
+  <si>
+    <t>Mini Batch
+5</t>
   </si>
   <si>
     <t>Master
-[1][2]</t>
+[1, 2]</t>
+  </si>
+  <si>
+    <t>Cross Ref [1, 2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Master
+[1, 2, 3, 4] </t>
+  </si>
+  <si>
+    <t>Cross Ref [1, 2, 3, 4]</t>
+  </si>
+  <si>
+    <t>Cross Ref [1, 2, 3, 4, 5]</t>
+  </si>
+  <si>
+    <t>Master
+[3, 4]</t>
+  </si>
+  <si>
+    <t>Cross Ref [3, 4]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,8 +155,42 @@
     </font>
     <font>
       <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="0" tint="-0.499984740745262"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -164,10 +198,30 @@
     <font>
       <b/>
       <sz val="14"/>
-      <color theme="1"/>
+      <color theme="0" tint="-0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -343,66 +397,90 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -428,13 +506,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>213360</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>172720</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -497,13 +575,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>71120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>659423</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>175846</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -550,13 +628,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>10160</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>58616</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>630116</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>142240</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -603,13 +681,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>864016</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>135328</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>644770</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>3123</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -656,13 +734,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>29309</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>644770</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>145737</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -709,13 +787,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>10160</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>132080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>650240</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>132080</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -762,13 +840,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>41640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>599440</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>10160</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -815,13 +893,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>20321</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>589280</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>62459</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -868,13 +946,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>39141</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>589280</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>39141</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -921,13 +999,13 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>999345</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>104098</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>10160</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -943,8 +1021,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14813197" y="2852295"/>
-          <a:ext cx="5142209" cy="1290820"/>
+          <a:off x="14762970" y="3279098"/>
+          <a:ext cx="5138565" cy="1483402"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -974,13 +1052,13 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>10409</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>787757</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>31230</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -996,8 +1074,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="14834016" y="4340902"/>
-          <a:ext cx="5107839" cy="2092377"/>
+          <a:off x="14790034" y="4953000"/>
+          <a:ext cx="5095348" cy="2602980"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -1027,13 +1105,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>81280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1083,13 +1161,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>375920</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>396240</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1138,13 +1216,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>10160</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1194,13 +1272,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>396240</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>71120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>71120</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1250,13 +1328,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>10160</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1306,13 +1384,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>386080</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>599440</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1362,13 +1440,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>396240</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>71120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>71120</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1418,13 +1496,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>221889</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>114301</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1237889</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>126024</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1512,13 +1590,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>729889</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>114301</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>729889</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>126024</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1573,13 +1651,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>221889</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>101112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1263289</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>101112</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1631,13 +1709,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>317500</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>63989</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>26865</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>75712</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1704,13 +1782,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>825500</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>63989</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>825500</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>75712</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1765,13 +1843,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>317500</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>52265</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1823,13 +1901,13 @@
     <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>363415</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>64814</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>1379415</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>76049</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1896,13 +1974,13 @@
     <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>871415</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>64814</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>871415</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>76049</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1957,13 +2035,13 @@
     <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>363415</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>51625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>1404815</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>51625</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2015,13 +2093,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>174626</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>71770</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>682626</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>31749</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2075,14 +2153,23 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" b="1"/>
+            <a:rPr lang="en-US" sz="1200" b="1">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
             <a:t>Cross</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" b="1" baseline="0"/>
+            <a:rPr lang="en-US" sz="1200" b="1" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
             <a:t> Reference at Depth 0</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1200" b="1"/>
+          <a:endParaRPr lang="en-US" sz="1200" b="1">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2092,13 +2179,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1444625</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>280867</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2145,13 +2232,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>29308</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>43962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>43962</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2198,13 +2285,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>49822</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>123094</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>592014</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>123094</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2251,13 +2338,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>41028</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>84995</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>583220</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>84995</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2304,13 +2391,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>46888</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>61552</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>589080</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>61552</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2357,13 +2444,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>23440</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>67414</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>565632</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>67414</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2410,13 +2497,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1306049</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>29991</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>443035</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>178581</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2479,13 +2566,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>1287488</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>29502</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>204666</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>1269</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2548,13 +2635,13 @@
     <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>1342196</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>29013</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
       <xdr:colOff>308220</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>7130</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2617,13 +2704,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1412876</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>680667</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>36642</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2675,13 +2762,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>670606</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>79491</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>378558</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>35944</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2730,13 +2817,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>715000</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>52115</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
       <xdr:colOff>407933</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>90000</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2787,14 +2874,14 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1412875</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>31752</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>779947</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>89730</xdr:rowOff>
+      <xdr:colOff>815203</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>89244</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2809,12 +2896,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="7778750" y="9207500"/>
-          <a:ext cx="1716572" cy="1581980"/>
+          <a:off x="8023740" y="10919428"/>
+          <a:ext cx="1751828" cy="1526573"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 39827"/>
+            <a:gd name="adj1" fmla="val 50000"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -2845,13 +2932,13 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>32522</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>714376</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2905,14 +2992,23 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" b="1"/>
+            <a:rPr lang="en-US" sz="1200" b="1">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
             <a:t>Cross</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" b="1" baseline="0"/>
+            <a:rPr lang="en-US" sz="1200" b="1" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
             <a:t> Reference at Depth 1</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1200" b="1"/>
+          <a:endParaRPr lang="en-US" sz="1200" b="1">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2922,13 +3018,13 @@
     <xdr:from>
       <xdr:col>22</xdr:col>
       <xdr:colOff>218187</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>69619</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>873125</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>111125</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2982,14 +3078,23 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" b="1"/>
+            <a:rPr lang="en-US" sz="1200" b="1">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
             <a:t>Cross</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" b="1" baseline="0"/>
+            <a:rPr lang="en-US" sz="1200" b="1" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
             <a:t> Reference at Depth 2</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1200" b="1"/>
+          <a:endParaRPr lang="en-US" sz="1200" b="1">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2998,9 +3103,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>197884</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>43380</xdr:rowOff>
+      <xdr:colOff>208125</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>12655</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3770866" cy="499367"/>
     <xdr:sp macro="" textlink="">
@@ -3016,7 +3121,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8241217" y="8100824"/>
+          <a:off x="8278770" y="8001365"/>
           <a:ext cx="3770866" cy="499367"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3047,7 +3152,14 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" sz="1300" i="1"/>
-            <a:t>Combined Cross-ref at Depth=1 updates original Cross-ref</a:t>
+            <a:t>Combined Cross-ref at Depth=1 updates </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1300" i="1"/>
+            <a:t>the original Cross-ref</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3057,9 +3169,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>858888</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>179873</xdr:rowOff>
+      <xdr:colOff>869130</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>149148</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3776611" cy="499367"/>
     <xdr:sp macro="" textlink="">
@@ -3075,7 +3187,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9593666" y="9888317"/>
+          <a:off x="9625985" y="9797051"/>
           <a:ext cx="3776611" cy="499367"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3106,7 +3218,14 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" sz="1300" i="1"/>
-            <a:t>Combined Cross-ref at Depth=2 updates original Cross-ref</a:t>
+            <a:t>Combined Cross-ref at Depth=2 updates </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1300" i="1"/>
+            <a:t>the original Cross-ref</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3117,7 +3236,7 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>697459</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>44115</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3890416" cy="511510"/>
@@ -3176,13 +3295,13 @@
     <xdr:from>
       <xdr:col>30</xdr:col>
       <xdr:colOff>432644</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>99125</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
       <xdr:colOff>227964</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>110848</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3249,13 +3368,13 @@
     <xdr:from>
       <xdr:col>31</xdr:col>
       <xdr:colOff>330304</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>99125</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
       <xdr:colOff>330304</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>110848</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3310,13 +3429,13 @@
     <xdr:from>
       <xdr:col>30</xdr:col>
       <xdr:colOff>419750</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>68207</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
       <xdr:colOff>240470</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>68207</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3368,13 +3487,13 @@
     <xdr:from>
       <xdr:col>29</xdr:col>
       <xdr:colOff>365124</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>33102</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
       <xdr:colOff>317499</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3428,14 +3547,23 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" b="1"/>
+            <a:rPr lang="en-US" sz="1200" b="1">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
             <a:t>Cross</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" b="1" baseline="0"/>
+            <a:rPr lang="en-US" sz="1200" b="1" baseline="0">
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
             <a:t> Reference at Depth 3</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1200" b="1"/>
+          <a:endParaRPr lang="en-US" sz="1200" b="1">
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -3445,13 +3573,13 @@
     <xdr:from>
       <xdr:col>25</xdr:col>
       <xdr:colOff>10410</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>10409</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>114509</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>41638</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3467,8 +3595,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="19955656" y="3945327"/>
-          <a:ext cx="978525" cy="624590"/>
+          <a:off x="19901785" y="4566534"/>
+          <a:ext cx="977224" cy="618604"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3523,13 +3651,22 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1">
+            <a:rPr lang="en-US" sz="1600" b="1">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
             <a:t>Site Master</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -3539,13 +3676,13 @@
     <xdr:from>
       <xdr:col>28</xdr:col>
       <xdr:colOff>311709</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>1445</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
       <xdr:colOff>311709</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3597,13 +3734,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>187378</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>93689</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>187378</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>176968</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3655,13 +3792,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>162811</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>6663</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>162811</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>6663</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3713,13 +3850,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>179883</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>179883</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>179883</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>13325</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3771,13 +3908,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>186545</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>155315</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>186545</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>19987</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3829,13 +3966,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>172388</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>120339</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>172388</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>172388</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3886,15 +4023,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>166558</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:colOff>79375</xdr:colOff>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1186722</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>145737</xdr:rowOff>
+      <xdr:rowOff>18737</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3909,8 +4046,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="166558" y="3175000"/>
-          <a:ext cx="1634344" cy="1311639"/>
+          <a:off x="79375" y="3714750"/>
+          <a:ext cx="1710597" cy="1510987"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -3964,21 +4101,25 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" baseline="0">
+            <a:rPr lang="en-US" sz="1600" b="1" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
-            <a:t>DATA SET OF SINGLE COUNTRY</a:t>
+            <a:t>DATA SET OF SINGLE BATCH</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0" i="1" baseline="0">
+            <a:rPr lang="en-US" sz="1600" b="0" i="1" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
             <a:t>#Records &gt; 5000</a:t>
           </a:r>
@@ -3986,10 +4127,12 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0" i="1" baseline="0">
+            <a:rPr lang="en-US" sz="1600" b="0" i="1" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:rPr>
             <a:t>ex: 20,100</a:t>
           </a:r>
@@ -4002,13 +4145,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>275319</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>172720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>718279</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>83279</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -4062,7 +4205,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>287755</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>149584</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1679731" cy="823649"/>
@@ -4425,10 +4568,10 @@
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="B3:AD38"/>
+  <dimension ref="B2:AE37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="45" zoomScaleNormal="45" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScale="43" zoomScaleNormal="43" workbookViewId="0">
+      <selection activeCell="AJ4" sqref="AJ4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4437,346 +4580,1235 @@
     <col min="4" max="4" width="14.6328125" customWidth="1"/>
     <col min="6" max="6" width="12.54296875" style="1" customWidth="1"/>
     <col min="7" max="7" width="3.1796875" customWidth="1"/>
-    <col min="8" max="8" width="5.90625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="9.08984375" style="2" customWidth="1"/>
     <col min="9" max="9" width="11.81640625" style="2" customWidth="1"/>
     <col min="10" max="10" width="23.81640625" customWidth="1"/>
     <col min="11" max="11" width="9.81640625" customWidth="1"/>
     <col min="12" max="12" width="12.6328125" customWidth="1"/>
     <col min="13" max="13" width="3.6328125" customWidth="1"/>
+    <col min="14" max="14" width="11.90625" customWidth="1"/>
     <col min="15" max="15" width="11.36328125" customWidth="1"/>
     <col min="17" max="17" width="18.6328125" customWidth="1"/>
     <col min="19" max="19" width="14.453125" customWidth="1"/>
     <col min="20" max="20" width="4.81640625" customWidth="1"/>
-    <col min="21" max="21" width="12.81640625" customWidth="1"/>
+    <col min="21" max="21" width="17.6328125" customWidth="1"/>
     <col min="22" max="22" width="13.453125" customWidth="1"/>
     <col min="24" max="24" width="22.1796875" customWidth="1"/>
     <col min="25" max="25" width="11.36328125" customWidth="1"/>
     <col min="26" max="26" width="12.453125" customWidth="1"/>
     <col min="27" max="27" width="4.90625" customWidth="1"/>
-    <col min="28" max="28" width="9.26953125" customWidth="1"/>
+    <col min="28" max="28" width="14.36328125" customWidth="1"/>
     <col min="29" max="29" width="9.08984375" customWidth="1"/>
     <col min="30" max="30" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:28" s="1" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="D3" s="22" t="s">
+    <row r="2" spans="3:31" s="9" customFormat="1" ht="20" x14ac:dyDescent="0.4">
+      <c r="D2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="L2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="S2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="Z2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+    </row>
+    <row r="3" spans="3:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
+      <c r="AA3" s="10"/>
+      <c r="AB3" s="10"/>
+      <c r="AC3" s="10"/>
+      <c r="AD3" s="10"/>
+      <c r="AE3" s="10"/>
+    </row>
+    <row r="4" spans="3:31" ht="13.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="10"/>
+      <c r="AA4" s="10"/>
+      <c r="AB4" s="10"/>
+      <c r="AC4" s="10"/>
+      <c r="AD4" s="10"/>
+      <c r="AE4" s="10"/>
+    </row>
+    <row r="5" spans="3:31" ht="18.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="C5" s="10"/>
+      <c r="D5" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="22" t="s">
+      <c r="I5" s="34"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10"/>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="10"/>
+      <c r="Z5" s="10"/>
+      <c r="AA5" s="10"/>
+      <c r="AB5" s="10"/>
+      <c r="AC5" s="10"/>
+      <c r="AD5" s="10"/>
+      <c r="AE5" s="10"/>
+    </row>
+    <row r="6" spans="3:31" ht="17.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C6" s="10"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="17"/>
+      <c r="U6" s="17"/>
+      <c r="V6" s="17"/>
+      <c r="W6" s="17"/>
+      <c r="X6" s="17"/>
+      <c r="Y6" s="17"/>
+      <c r="Z6" s="17"/>
+      <c r="AA6" s="17"/>
+      <c r="AB6" s="17"/>
+      <c r="AC6" s="17"/>
+      <c r="AD6" s="17"/>
+      <c r="AE6" s="17"/>
+    </row>
+    <row r="7" spans="3:31" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C7" s="10"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="17"/>
+      <c r="T7" s="17"/>
+      <c r="U7" s="17"/>
+      <c r="V7" s="17"/>
+      <c r="W7" s="17"/>
+      <c r="X7" s="17"/>
+      <c r="Y7" s="17"/>
+      <c r="Z7" s="17"/>
+      <c r="AA7" s="17"/>
+      <c r="AB7" s="17"/>
+      <c r="AC7" s="17"/>
+      <c r="AD7" s="17"/>
+      <c r="AE7" s="17"/>
+    </row>
+    <row r="8" spans="3:31" ht="19" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="17"/>
+      <c r="Q8" s="17"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="17"/>
+      <c r="U8" s="17"/>
+      <c r="V8" s="17"/>
+      <c r="W8" s="17"/>
+      <c r="X8" s="17"/>
+      <c r="Y8" s="17"/>
+      <c r="Z8" s="17"/>
+      <c r="AA8" s="17"/>
+      <c r="AB8" s="17"/>
+      <c r="AC8" s="17"/>
+      <c r="AD8" s="17"/>
+      <c r="AE8" s="17"/>
+    </row>
+    <row r="9" spans="3:31" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="17"/>
+      <c r="S9" s="17"/>
+      <c r="T9" s="17"/>
+      <c r="U9" s="17"/>
+      <c r="V9" s="17"/>
+      <c r="W9" s="17"/>
+      <c r="X9" s="17"/>
+      <c r="Y9" s="17"/>
+      <c r="Z9" s="17"/>
+      <c r="AA9" s="17"/>
+      <c r="AB9" s="17"/>
+      <c r="AC9" s="17"/>
+      <c r="AD9" s="17"/>
+      <c r="AE9" s="17"/>
+    </row>
+    <row r="10" spans="3:31" ht="20.5" x14ac:dyDescent="0.45">
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="O10" s="35"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="17"/>
+      <c r="T10" s="17"/>
+      <c r="U10" s="17"/>
+      <c r="V10" s="17"/>
+      <c r="W10" s="17"/>
+      <c r="X10" s="17"/>
+      <c r="Y10" s="17"/>
+      <c r="Z10" s="17"/>
+      <c r="AA10" s="17"/>
+      <c r="AB10" s="17"/>
+      <c r="AC10" s="17"/>
+      <c r="AD10" s="17"/>
+      <c r="AE10" s="17"/>
+    </row>
+    <row r="11" spans="3:31" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="17"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="17"/>
+      <c r="U11" s="17"/>
+      <c r="V11" s="17"/>
+      <c r="W11" s="17"/>
+      <c r="X11" s="17"/>
+      <c r="Y11" s="17"/>
+      <c r="Z11" s="17"/>
+      <c r="AA11" s="17"/>
+      <c r="AB11" s="17"/>
+      <c r="AC11" s="17"/>
+      <c r="AD11" s="17"/>
+      <c r="AE11" s="17"/>
+    </row>
+    <row r="12" spans="3:31" ht="19" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="C12" s="10"/>
+      <c r="D12" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="10"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="17"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="17"/>
+      <c r="U12" s="17"/>
+      <c r="V12" s="17"/>
+      <c r="W12" s="17"/>
+      <c r="X12" s="17"/>
+      <c r="Y12" s="17"/>
+      <c r="Z12" s="17"/>
+      <c r="AA12" s="17"/>
+      <c r="AB12" s="17"/>
+      <c r="AC12" s="17"/>
+      <c r="AD12" s="17"/>
+      <c r="AE12" s="17"/>
+    </row>
+    <row r="13" spans="3:31" ht="20.5" x14ac:dyDescent="0.45">
+      <c r="C13" s="10"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="22" t="s">
+      <c r="I13" s="34"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="17"/>
+      <c r="P13" s="17"/>
+      <c r="Q13" s="17"/>
+      <c r="R13" s="17"/>
+      <c r="S13" s="17"/>
+      <c r="T13" s="17"/>
+      <c r="U13" s="17"/>
+      <c r="V13" s="17"/>
+      <c r="W13" s="17"/>
+      <c r="X13" s="17"/>
+      <c r="Y13" s="17"/>
+      <c r="Z13" s="17"/>
+      <c r="AA13" s="17"/>
+      <c r="AB13" s="17"/>
+      <c r="AC13" s="17"/>
+      <c r="AD13" s="17"/>
+      <c r="AE13" s="17"/>
+    </row>
+    <row r="14" spans="3:31" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C14" s="10"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="17"/>
+      <c r="S14" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="T14" s="17"/>
+      <c r="U14" s="17"/>
+      <c r="V14" s="17"/>
+      <c r="W14" s="17"/>
+      <c r="X14" s="17"/>
+      <c r="Y14" s="17"/>
+      <c r="Z14" s="17"/>
+      <c r="AA14" s="17"/>
+      <c r="AB14" s="17"/>
+      <c r="AC14" s="17"/>
+      <c r="AD14" s="17"/>
+      <c r="AE14" s="17"/>
+    </row>
+    <row r="15" spans="3:31" ht="18.649999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="17"/>
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17"/>
+      <c r="R15" s="17"/>
+      <c r="S15" s="13"/>
+      <c r="T15" s="17"/>
+      <c r="U15" s="17"/>
+      <c r="V15" s="17"/>
+      <c r="W15" s="17"/>
+      <c r="X15" s="17"/>
+      <c r="Y15" s="17"/>
+      <c r="Z15" s="17"/>
+      <c r="AA15" s="17"/>
+      <c r="AB15" s="17"/>
+      <c r="AC15" s="17"/>
+      <c r="AD15" s="17"/>
+      <c r="AE15" s="17"/>
+    </row>
+    <row r="16" spans="3:31" ht="20.5" x14ac:dyDescent="0.45">
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+      <c r="P16" s="17"/>
+      <c r="Q16" s="17"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="17"/>
+      <c r="U16" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="V16" s="35"/>
+      <c r="W16" s="17"/>
+      <c r="X16" s="17"/>
+      <c r="Y16" s="17"/>
+      <c r="Z16" s="17"/>
+      <c r="AA16" s="17"/>
+      <c r="AB16" s="17"/>
+      <c r="AC16" s="17"/>
+      <c r="AD16" s="17"/>
+      <c r="AE16" s="17"/>
+    </row>
+    <row r="17" spans="2:31" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="17"/>
+      <c r="T17" s="17"/>
+      <c r="U17" s="19"/>
+      <c r="V17" s="19"/>
+      <c r="W17" s="17"/>
+      <c r="X17" s="17"/>
+      <c r="Y17" s="17"/>
+      <c r="Z17" s="17"/>
+      <c r="AA17" s="17"/>
+      <c r="AB17" s="17"/>
+      <c r="AC17" s="17"/>
+      <c r="AD17" s="17"/>
+      <c r="AE17" s="17"/>
+    </row>
+    <row r="18" spans="2:31" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B18" s="4"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="17"/>
+      <c r="T18" s="17"/>
+      <c r="U18" s="19"/>
+      <c r="V18" s="19"/>
+      <c r="W18" s="17"/>
+      <c r="X18" s="17"/>
+      <c r="Y18" s="17"/>
+      <c r="Z18" s="17"/>
+      <c r="AA18" s="17"/>
+      <c r="AB18" s="17"/>
+      <c r="AC18" s="17"/>
+      <c r="AD18" s="17"/>
+      <c r="AE18" s="17"/>
+    </row>
+    <row r="19" spans="2:31" ht="19" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B19" s="4"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="10"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="17"/>
+      <c r="Q19" s="17"/>
+      <c r="R19" s="17"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="17"/>
+      <c r="U19" s="17"/>
+      <c r="V19" s="17"/>
+      <c r="W19" s="17"/>
+      <c r="X19" s="17"/>
+      <c r="Y19" s="17"/>
+      <c r="Z19" s="17"/>
+      <c r="AA19" s="17"/>
+      <c r="AB19" s="17"/>
+      <c r="AC19" s="17"/>
+      <c r="AD19" s="17"/>
+      <c r="AE19" s="17"/>
+    </row>
+    <row r="20" spans="2:31" ht="20.5" x14ac:dyDescent="0.45">
+      <c r="B20" s="4"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="I20" s="35"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="17"/>
+      <c r="O20" s="17"/>
+      <c r="P20" s="17"/>
+      <c r="Q20" s="17"/>
+      <c r="R20" s="17"/>
+      <c r="S20" s="17"/>
+      <c r="T20" s="17"/>
+      <c r="U20" s="17"/>
+      <c r="V20" s="17"/>
+      <c r="W20" s="17"/>
+      <c r="X20" s="17"/>
+      <c r="Y20" s="17"/>
+      <c r="Z20" s="17"/>
+      <c r="AA20" s="17"/>
+      <c r="AB20" s="17"/>
+      <c r="AC20" s="17"/>
+      <c r="AD20" s="17"/>
+      <c r="AE20" s="17"/>
+    </row>
+    <row r="21" spans="2:31" ht="26" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B21" s="4"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="17"/>
+      <c r="Q21" s="17"/>
+      <c r="R21" s="17"/>
+      <c r="S21" s="17"/>
+      <c r="T21" s="17"/>
+      <c r="U21" s="17"/>
+      <c r="V21" s="17"/>
+      <c r="W21" s="17"/>
+      <c r="X21" s="17"/>
+      <c r="Y21" s="17"/>
+      <c r="Z21" s="21"/>
+      <c r="AA21" s="17"/>
+      <c r="AB21" s="17"/>
+      <c r="AC21" s="17"/>
+      <c r="AD21" s="17"/>
+      <c r="AE21" s="17"/>
+    </row>
+    <row r="22" spans="2:31" ht="23" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B22" s="4"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="17"/>
+      <c r="P22" s="17"/>
+      <c r="Q22" s="17"/>
+      <c r="R22" s="17"/>
+      <c r="S22" s="17"/>
+      <c r="T22" s="17"/>
+      <c r="U22" s="17"/>
+      <c r="V22" s="17"/>
+      <c r="W22" s="17"/>
+      <c r="X22" s="17"/>
+      <c r="Y22" s="17"/>
+      <c r="Z22" s="21"/>
+      <c r="AA22" s="17"/>
+      <c r="AB22" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC22" s="36"/>
+      <c r="AD22" s="34"/>
+      <c r="AE22" s="17"/>
+    </row>
+    <row r="23" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B23" s="4"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="M23" s="17"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="17"/>
+      <c r="P23" s="17"/>
+      <c r="Q23" s="17"/>
+      <c r="R23" s="17"/>
+      <c r="S23" s="17"/>
+      <c r="T23" s="17"/>
+      <c r="U23" s="17"/>
+      <c r="V23" s="17"/>
+      <c r="W23" s="17"/>
+      <c r="X23" s="17"/>
+      <c r="Y23" s="17"/>
+      <c r="Z23" s="21"/>
+      <c r="AA23" s="17"/>
+      <c r="AB23" s="22"/>
+      <c r="AC23" s="23"/>
+      <c r="AD23" s="24"/>
+      <c r="AE23" s="17"/>
+    </row>
+    <row r="24" spans="2:31" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="17"/>
+      <c r="O24" s="17"/>
+      <c r="P24" s="17"/>
+      <c r="Q24" s="17"/>
+      <c r="R24" s="17"/>
+      <c r="S24" s="17"/>
+      <c r="T24" s="17"/>
+      <c r="U24" s="17"/>
+      <c r="V24" s="17"/>
+      <c r="W24" s="17"/>
+      <c r="X24" s="17"/>
+      <c r="Y24" s="17"/>
+      <c r="Z24" s="17"/>
+      <c r="AA24" s="17"/>
+      <c r="AB24" s="22"/>
+      <c r="AC24" s="23"/>
+      <c r="AD24" s="24"/>
+      <c r="AE24" s="17"/>
+    </row>
+    <row r="25" spans="2:31" ht="21" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="30"/>
+      <c r="M25" s="17"/>
+      <c r="N25" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="O25" s="35"/>
+      <c r="P25" s="17"/>
+      <c r="Q25" s="17"/>
+      <c r="R25" s="17"/>
+      <c r="S25" s="17"/>
+      <c r="T25" s="17"/>
+      <c r="U25" s="17"/>
+      <c r="V25" s="17"/>
+      <c r="W25" s="17"/>
+      <c r="X25" s="17"/>
+      <c r="Y25" s="17"/>
+      <c r="Z25" s="17"/>
+      <c r="AA25" s="17"/>
+      <c r="AB25" s="17"/>
+      <c r="AC25" s="17"/>
+      <c r="AD25" s="17"/>
+      <c r="AE25" s="17"/>
+    </row>
+    <row r="26" spans="2:31" ht="19" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="C26" s="10"/>
+      <c r="D26" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" s="10"/>
+      <c r="F26" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="10"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="17"/>
+      <c r="Q26" s="17"/>
+      <c r="R26" s="17"/>
+      <c r="S26" s="17"/>
+      <c r="T26" s="17"/>
+      <c r="U26" s="17"/>
+      <c r="V26" s="17"/>
+      <c r="W26" s="17"/>
+      <c r="X26" s="17"/>
+      <c r="Y26" s="17"/>
+      <c r="Z26" s="17"/>
+      <c r="AA26" s="17"/>
+      <c r="AB26" s="17"/>
+      <c r="AC26" s="17"/>
+      <c r="AD26" s="17"/>
+      <c r="AE26" s="17"/>
+    </row>
+    <row r="27" spans="2:31" ht="20.5" x14ac:dyDescent="0.45">
+      <c r="C27" s="10"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="T3" s="22"/>
-      <c r="U3" s="22"/>
-      <c r="V3" s="22"/>
-      <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="22" t="s">
-        <v>10</v>
+      <c r="I27" s="35"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="17"/>
+      <c r="Q27" s="17"/>
+      <c r="R27" s="17"/>
+      <c r="S27" s="17"/>
+      <c r="T27" s="17"/>
+      <c r="U27" s="17"/>
+      <c r="V27" s="17"/>
+      <c r="W27" s="17"/>
+      <c r="X27" s="17"/>
+      <c r="Y27" s="17"/>
+      <c r="Z27" s="17"/>
+      <c r="AA27" s="17"/>
+      <c r="AB27" s="17"/>
+      <c r="AC27" s="17"/>
+      <c r="AD27" s="17"/>
+      <c r="AE27" s="17"/>
+    </row>
+    <row r="28" spans="2:31" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C28" s="10"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="17"/>
+      <c r="K28" s="17"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="17"/>
+      <c r="N28" s="17"/>
+      <c r="O28" s="17"/>
+      <c r="P28" s="17"/>
+      <c r="Q28" s="17"/>
+      <c r="R28" s="17"/>
+      <c r="S28" s="17"/>
+      <c r="T28" s="17"/>
+      <c r="U28" s="17"/>
+      <c r="V28" s="17"/>
+      <c r="W28" s="17"/>
+      <c r="X28" s="17"/>
+      <c r="Y28" s="17"/>
+      <c r="Z28" s="17"/>
+      <c r="AA28" s="17"/>
+      <c r="AB28" s="17"/>
+      <c r="AC28" s="17"/>
+      <c r="AD28" s="17"/>
+      <c r="AE28" s="17"/>
+    </row>
+    <row r="29" spans="2:31" ht="19" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="17"/>
+      <c r="O29" s="17"/>
+      <c r="P29" s="17"/>
+      <c r="Q29" s="17"/>
+      <c r="R29" s="17"/>
+      <c r="S29" s="17"/>
+      <c r="T29" s="17"/>
+      <c r="U29" s="17"/>
+      <c r="V29" s="17"/>
+      <c r="W29" s="17"/>
+      <c r="X29" s="17"/>
+      <c r="Y29" s="17"/>
+      <c r="Z29" s="17"/>
+      <c r="AA29" s="17"/>
+      <c r="AB29" s="17"/>
+      <c r="AC29" s="17"/>
+      <c r="AD29" s="17"/>
+      <c r="AE29" s="17"/>
+    </row>
+    <row r="30" spans="2:31" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="17"/>
+      <c r="N30" s="17"/>
+      <c r="O30" s="17"/>
+      <c r="P30" s="17"/>
+      <c r="Q30" s="17"/>
+      <c r="R30" s="17"/>
+      <c r="S30" s="17"/>
+      <c r="T30" s="17"/>
+      <c r="U30" s="17"/>
+      <c r="V30" s="17"/>
+      <c r="W30" s="17"/>
+      <c r="X30" s="17"/>
+      <c r="Y30" s="17"/>
+      <c r="Z30" s="17"/>
+      <c r="AA30" s="17"/>
+      <c r="AB30" s="17"/>
+      <c r="AC30" s="17"/>
+      <c r="AD30" s="17"/>
+      <c r="AE30" s="17"/>
+    </row>
+    <row r="31" spans="2:31" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
+      <c r="L31" s="17"/>
+      <c r="M31" s="17"/>
+      <c r="N31" s="17"/>
+      <c r="O31" s="17"/>
+      <c r="P31" s="17"/>
+      <c r="Q31" s="17"/>
+      <c r="R31" s="17"/>
+      <c r="S31" s="17"/>
+      <c r="T31" s="17"/>
+      <c r="U31" s="17"/>
+      <c r="V31" s="17"/>
+      <c r="W31" s="17"/>
+      <c r="X31" s="17"/>
+      <c r="Y31" s="17"/>
+      <c r="Z31" s="17"/>
+      <c r="AA31" s="17"/>
+      <c r="AB31" s="17"/>
+      <c r="AC31" s="17"/>
+      <c r="AD31" s="17"/>
+      <c r="AE31" s="17"/>
+    </row>
+    <row r="32" spans="2:31" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="17"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="17"/>
+      <c r="O32" s="17"/>
+      <c r="P32" s="17"/>
+      <c r="Q32" s="17"/>
+      <c r="R32" s="17"/>
+      <c r="S32" s="17"/>
+      <c r="T32" s="17"/>
+      <c r="U32" s="17"/>
+      <c r="V32" s="17"/>
+      <c r="W32" s="17"/>
+      <c r="X32" s="17"/>
+      <c r="Y32" s="17"/>
+      <c r="Z32" s="17"/>
+      <c r="AA32" s="17"/>
+      <c r="AB32" s="17"/>
+      <c r="AC32" s="17"/>
+      <c r="AD32" s="17"/>
+      <c r="AE32" s="17"/>
+    </row>
+    <row r="33" spans="3:31" ht="19" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="C33" s="10"/>
+      <c r="D33" s="25" t="s">
+        <v>19</v>
       </c>
-      <c r="AA3" s="22"/>
-      <c r="AB3" s="22"/>
-    </row>
-    <row r="4" spans="4:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="4:28" ht="13.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="F5" s="14" t="s">
-        <v>18</v>
+      <c r="E33" s="10"/>
+      <c r="F33" s="28" t="s">
+        <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="4:28" ht="13.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="D6" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="15"/>
-      <c r="H6" s="13" t="s">
+      <c r="G33" s="10"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="17"/>
+      <c r="L33" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="13"/>
+      <c r="M33" s="17"/>
+      <c r="N33" s="17"/>
+      <c r="O33" s="17"/>
+      <c r="P33" s="17"/>
+      <c r="Q33" s="17"/>
+      <c r="R33" s="17"/>
+      <c r="S33" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="T33" s="17"/>
+      <c r="U33" s="17"/>
+      <c r="V33" s="17"/>
+      <c r="W33" s="17"/>
+      <c r="X33" s="17"/>
+      <c r="Y33" s="17"/>
+      <c r="Z33" s="17"/>
+      <c r="AA33" s="17"/>
+      <c r="AB33" s="17"/>
+      <c r="AC33" s="17"/>
+      <c r="AD33" s="17"/>
+      <c r="AE33" s="17"/>
     </row>
-    <row r="7" spans="4:28" ht="14.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D7" s="18"/>
-      <c r="F7" s="16"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="12"/>
-    </row>
-    <row r="8" spans="4:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D8" s="19"/>
-      <c r="F8" s="10"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="12"/>
-    </row>
-    <row r="9" spans="4:28" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="L9" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="4:28" x14ac:dyDescent="0.35">
-      <c r="L10" s="15"/>
-    </row>
-    <row r="11" spans="4:28" x14ac:dyDescent="0.35">
-      <c r="L11" s="16"/>
-      <c r="N11" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="O11" s="13"/>
-    </row>
-    <row r="12" spans="4:28" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-    </row>
-    <row r="13" spans="4:28" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="D13" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-    </row>
-    <row r="14" spans="4:28" x14ac:dyDescent="0.35">
-      <c r="D14" s="18"/>
-      <c r="F14" s="15"/>
-      <c r="H14" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="I14" s="24"/>
-    </row>
-    <row r="15" spans="4:28" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D15" s="19"/>
-      <c r="F15" s="16"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="12"/>
-      <c r="S15" s="14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="4:28" ht="18.649999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="H16" s="11"/>
-      <c r="I16" s="12"/>
-      <c r="S16" s="15"/>
-    </row>
-    <row r="17" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="S17" s="16"/>
-      <c r="U17" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="V17" s="13"/>
-    </row>
-    <row r="18" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="L18" s="3"/>
-      <c r="U18" s="6"/>
-      <c r="V18" s="6"/>
-    </row>
-    <row r="19" spans="2:30" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="21"/>
-      <c r="U19" s="6"/>
-      <c r="V19" s="6"/>
-    </row>
-    <row r="20" spans="2:30" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="21"/>
-      <c r="D20" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="B21" s="21"/>
-      <c r="D21" s="18"/>
-      <c r="F21" s="15"/>
-      <c r="H21" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="I21" s="13"/>
-    </row>
-    <row r="22" spans="2:30" ht="16.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="21"/>
-      <c r="D22" s="19"/>
-      <c r="F22" s="16"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="12"/>
-      <c r="Z22" s="20"/>
-    </row>
-    <row r="23" spans="2:30" ht="15.65" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="21"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="12"/>
-      <c r="Z23" s="20"/>
-      <c r="AB23" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="AC23" s="9"/>
-      <c r="AD23" s="9"/>
-    </row>
-    <row r="24" spans="2:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="21"/>
-      <c r="L24" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z24" s="20"/>
-      <c r="AB24" s="4"/>
-      <c r="AC24" s="7"/>
-      <c r="AD24" s="5"/>
-    </row>
-    <row r="25" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="L25" s="15"/>
-      <c r="AB25" s="4"/>
-      <c r="AC25" s="7"/>
-      <c r="AD25" s="5"/>
-    </row>
-    <row r="26" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="L26" s="16"/>
-      <c r="N26" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="O26" s="13"/>
-    </row>
-    <row r="27" spans="2:30" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="D27" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="N27" s="6"/>
-      <c r="O27" s="6"/>
-    </row>
-    <row r="28" spans="2:30" x14ac:dyDescent="0.35">
-      <c r="D28" s="18"/>
-      <c r="F28" s="15"/>
-      <c r="H28" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="I28" s="13"/>
-      <c r="N28" s="6"/>
-      <c r="O28" s="6"/>
-    </row>
-    <row r="29" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D29" s="19"/>
-      <c r="F29" s="16"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="12"/>
-    </row>
-    <row r="30" spans="2:30" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="H30" s="11"/>
-      <c r="I30" s="12"/>
-    </row>
-    <row r="33" spans="4:22" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="34" spans="4:22" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="D34" s="17" t="s">
+    <row r="34" spans="3:31" ht="20.5" x14ac:dyDescent="0.45">
+      <c r="C34" s="10"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F34" s="14" t="s">
-        <v>23</v>
+      <c r="I34" s="35"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="17"/>
+      <c r="L34" s="29"/>
+      <c r="M34" s="17"/>
+      <c r="N34" s="17"/>
+      <c r="O34" s="17"/>
+      <c r="P34" s="17"/>
+      <c r="Q34" s="17"/>
+      <c r="R34" s="17"/>
+      <c r="S34" s="29"/>
+      <c r="T34" s="17"/>
+      <c r="U34" s="17"/>
+      <c r="V34" s="17"/>
+      <c r="W34" s="17"/>
+      <c r="X34" s="17"/>
+      <c r="Y34" s="17"/>
+      <c r="Z34" s="17"/>
+      <c r="AA34" s="17"/>
+      <c r="AB34" s="17"/>
+      <c r="AC34" s="17"/>
+      <c r="AD34" s="17"/>
+      <c r="AE34" s="17"/>
+    </row>
+    <row r="35" spans="3:31" ht="24.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C35" s="10"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="17"/>
+      <c r="L35" s="30"/>
+      <c r="M35" s="17"/>
+      <c r="N35" s="35" t="s">
+        <v>4</v>
       </c>
-      <c r="L34" s="14" t="s">
-        <v>24</v>
+      <c r="O35" s="35"/>
+      <c r="P35" s="17"/>
+      <c r="Q35" s="17"/>
+      <c r="R35" s="17"/>
+      <c r="S35" s="30"/>
+      <c r="T35" s="17"/>
+      <c r="U35" s="35" t="s">
+        <v>4</v>
       </c>
-      <c r="S34" s="14" t="s">
-        <v>24</v>
-      </c>
+      <c r="V35" s="35"/>
+      <c r="W35" s="17"/>
+      <c r="X35" s="17"/>
+      <c r="Y35" s="17"/>
+      <c r="Z35" s="17"/>
+      <c r="AA35" s="17"/>
+      <c r="AB35" s="17"/>
+      <c r="AC35" s="17"/>
+      <c r="AD35" s="17"/>
+      <c r="AE35" s="17"/>
     </row>
-    <row r="35" spans="4:22" x14ac:dyDescent="0.35">
-      <c r="D35" s="18"/>
-      <c r="F35" s="15"/>
-      <c r="H35" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="I35" s="13"/>
-      <c r="L35" s="15"/>
-      <c r="S35" s="15"/>
+    <row r="36" spans="3:31" ht="19" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="17"/>
+      <c r="L36" s="17"/>
+      <c r="M36" s="17"/>
+      <c r="N36" s="19"/>
+      <c r="O36" s="19"/>
+      <c r="P36" s="17"/>
+      <c r="Q36" s="17"/>
+      <c r="R36" s="17"/>
+      <c r="S36" s="17"/>
+      <c r="T36" s="17"/>
+      <c r="U36" s="19"/>
+      <c r="V36" s="19"/>
+      <c r="W36" s="17"/>
+      <c r="X36" s="17"/>
+      <c r="Y36" s="17"/>
+      <c r="Z36" s="17"/>
+      <c r="AA36" s="17"/>
+      <c r="AB36" s="17"/>
+      <c r="AC36" s="17"/>
+      <c r="AD36" s="17"/>
+      <c r="AE36" s="17"/>
     </row>
-    <row r="36" spans="4:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D36" s="19"/>
-      <c r="F36" s="16"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="12"/>
-      <c r="L36" s="16"/>
-      <c r="N36" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="O36" s="13"/>
-      <c r="S36" s="16"/>
-      <c r="U36" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="V36" s="13"/>
-    </row>
-    <row r="37" spans="4:22" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="H37" s="11"/>
-      <c r="I37" s="12"/>
+    <row r="37" spans="3:31" x14ac:dyDescent="0.35">
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
       <c r="N37" s="6"/>
       <c r="O37" s="6"/>
+      <c r="P37" s="5"/>
+      <c r="Q37" s="5"/>
+      <c r="R37" s="5"/>
+      <c r="S37" s="5"/>
+      <c r="T37" s="5"/>
       <c r="U37" s="6"/>
       <c r="V37" s="6"/>
-    </row>
-    <row r="38" spans="4:22" x14ac:dyDescent="0.35">
-      <c r="N38" s="6"/>
-      <c r="O38" s="6"/>
-      <c r="U38" s="6"/>
-      <c r="V38" s="6"/>
+      <c r="W37" s="5"/>
+      <c r="X37" s="5"/>
+      <c r="Y37" s="5"/>
+      <c r="Z37" s="5"/>
+      <c r="AA37" s="5"/>
+      <c r="AB37" s="5"/>
+      <c r="AC37" s="5"/>
+      <c r="AD37" s="5"/>
+      <c r="AE37" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="Z22:Z24"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="B19:B24"/>
-    <mergeCell ref="D3:I3"/>
-    <mergeCell ref="L3:O3"/>
-    <mergeCell ref="S3:V3"/>
-    <mergeCell ref="Z3:AB3"/>
-    <mergeCell ref="D6:D8"/>
+  <mergeCells count="42">
+    <mergeCell ref="H36:I36"/>
     <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
     <mergeCell ref="H14:I14"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="F13:F15"/>
-    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="H15:I15"/>
     <mergeCell ref="H21:I21"/>
-    <mergeCell ref="D34:D36"/>
-    <mergeCell ref="F34:F36"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="L9:L11"/>
-    <mergeCell ref="L24:L26"/>
-    <mergeCell ref="L34:L36"/>
-    <mergeCell ref="F27:F29"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="N35:O35"/>
+    <mergeCell ref="S14:S16"/>
+    <mergeCell ref="U16:V16"/>
+    <mergeCell ref="S33:S35"/>
+    <mergeCell ref="U35:V35"/>
+    <mergeCell ref="D33:D35"/>
+    <mergeCell ref="F33:F35"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="L8:L10"/>
+    <mergeCell ref="L23:L25"/>
+    <mergeCell ref="L33:L35"/>
+    <mergeCell ref="F26:F28"/>
+    <mergeCell ref="H27:I27"/>
     <mergeCell ref="H28:I28"/>
     <mergeCell ref="H29:I29"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="D27:D29"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="N36:O36"/>
-    <mergeCell ref="S15:S17"/>
-    <mergeCell ref="U17:V17"/>
-    <mergeCell ref="S34:S36"/>
-    <mergeCell ref="U36:V36"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="Z21:Z23"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="D2:I2"/>
+    <mergeCell ref="L2:O2"/>
+    <mergeCell ref="S2:V2"/>
+    <mergeCell ref="Z2:AB2"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="AB22:AD22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4785,6 +5817,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100381A4B0C69D1B74E930075773FE831E5" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c66c8be124e052daf9738f504812c4f4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0d653d82-5b12-4c25-adbe-d06d43403509" xmlns:ns3="d27e8510-15d0-4d8d-9abc-9211c5595251" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="af3b9724c27eeb413420b342992812fc" ns2:_="" ns3:_="">
     <xsd:import namespace="0d653d82-5b12-4c25-adbe-d06d43403509"/>
@@ -4995,12 +6033,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5011,6 +6043,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AD19A22-0972-4F13-846C-03AE734CE31D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="d27e8510-15d0-4d8d-9abc-9211c5595251"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="0d653d82-5b12-4c25-adbe-d06d43403509"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A49B8509-A163-48C9-B276-99DB8BF8932D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5029,23 +6078,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AD19A22-0972-4F13-846C-03AE734CE31D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="d27e8510-15d0-4d8d-9abc-9211c5595251"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="0d653d82-5b12-4c25-adbe-d06d43403509"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51961439-86AC-40B2-BAEC-EA2E6A341226}">
   <ds:schemaRefs>

</xml_diff>